<commit_message>
Neuste Version des Workspaces und der App und Änderrungen an den PM_Sheets   -Hamzic
</commit_message>
<xml_diff>
--- a/PM-Sheets (Easter)/PM-Sheet_BAUX(1).xlsx
+++ b/PM-Sheets (Easter)/PM-Sheet_BAUX(1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr codeName="DieseArbeitsmappe" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armin\Desktop\PM-Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armin\Desktop\project-proposal-baux\PM-Sheets (Easter)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE86CA9E-5299-4A6A-9B86-DBAC4E592FB3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B250FE2-BFE0-444D-82C7-C7DCAF9557DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -868,7 +868,7 @@
   <dimension ref="B1:I16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1018,7 +1018,7 @@
     </row>
     <row r="13" spans="2:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>

</xml_diff>